<commit_message>
Add service, request functionality
</commit_message>
<xml_diff>
--- a/time.xlsx
+++ b/time.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Дата</t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>Всего потратил времени</t>
+  </si>
+  <si>
+    <t>Сделал простой сервис, раскидал по папкам файлы.</t>
   </si>
 </sst>
 </file>
@@ -384,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,7 +427,18 @@
       </c>
       <c r="F2" s="2">
         <f>SUM(B:B)</f>
-        <v>6.5</v>
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>44312</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add login validation, add local srorage
</commit_message>
<xml_diff>
--- a/time.xlsx
+++ b/time.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Дата</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>Сделал простой сервис, раскидал по папкам файлы.</t>
+  </si>
+  <si>
+    <t>Сделалсохранение в локал стор, добавил валидацию на странице логина.</t>
   </si>
 </sst>
 </file>
@@ -387,7 +390,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
@@ -427,7 +430,7 @@
       </c>
       <c r="F2" s="2">
         <f>SUM(B:B)</f>
-        <v>10.5</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -439,6 +442,17 @@
       </c>
       <c r="C3" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>44313</v>
+      </c>
+      <c r="B4">
+        <v>6.5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add guards, connect to REST API, request page
</commit_message>
<xml_diff>
--- a/time.xlsx
+++ b/time.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Дата</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>Сделалсохранение в локал стор, добавил валидацию на странице логина.</t>
+  </si>
+  <si>
+    <t>Сделал guards-ы, страницу просмотра заявки, получение данных с стороннего REST api.</t>
   </si>
 </sst>
 </file>
@@ -390,10 +393,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,7 +433,7 @@
       </c>
       <c r="F2" s="2">
         <f>SUM(B:B)</f>
-        <v>17</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -453,6 +456,17 @@
       </c>
       <c r="C4" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>44314</v>
+      </c>
+      <c r="B5">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finish validation to form
</commit_message>
<xml_diff>
--- a/time.xlsx
+++ b/time.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Дата</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>Сделал guards-ы, страницу просмотра заявки, получение данных с стороннего REST api.</t>
+  </si>
+  <si>
+    <t>Сверстал страницы, добавил валидацию полей для создания заявки.</t>
+  </si>
+  <si>
+    <t>Закончил валидацию полей на странице создания заявки.</t>
   </si>
 </sst>
 </file>
@@ -393,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -433,7 +439,7 @@
       </c>
       <c r="F2" s="2">
         <f>SUM(B:B)</f>
-        <v>22</v>
+        <v>28.75</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -467,6 +473,28 @@
       </c>
       <c r="C5" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>44315</v>
+      </c>
+      <c r="B6">
+        <v>5.25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>44316</v>
+      </c>
+      <c r="B7">
+        <v>1.5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>